<commit_message>
added casefile details 2 tc
</commit_message>
<xml_diff>
--- a/OutputFiles/TC25_Canine_Filter_Breed-Greyhnd_Neo4jData.xlsx
+++ b/OutputFiles/TC25_Canine_Filter_Breed-Greyhnd_Neo4jData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="54">
   <si>
     <t>Case ID</t>
   </si>
@@ -181,6 +181,20 @@
   </si>
   <si>
     <t>MATCH (f:file)-[*]-&gt;(c:case) WITH DISTINCT(f) AS f, c MATCH (f)--&gt;(parent) WHERE c.case_id IN ['NCATS-COP01CCB050022'] RETURN f.file_name AS `File Name` ,f.file_type AS `File Type`,head(labels(parent)) AS `Association`, f.file_description AS `Description`,f.file_format AS Format,((f.file_size)/1024) AS Size</t>
+  </si>
+  <si>
+    <t>105.75 KB</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)-[*]-&gt;(c:case) WITH DISTINCT(f) AS f, c MATCH (f)--&gt;(parent)
+WHERE c.case_id IN ['NCATS-COP01CCB050022']
+WITH
+['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+toInteger(floor(log(f.file_size)/log(1024))) as i,
+2 as precision,
+f,parent
+WITH f.file_size /(1024^i) AS value, 10^precision AS factor, units[i] as unit,f,parent
+RETURN f.file_name AS `File Name` ,f.file_type AS `File Type`,head(labels(parent)) AS `Association`, f.file_description AS `Description`,f.file_format AS Format,round(factor * value)/factor+ +unit AS Size</t>
   </si>
 </sst>
 </file>
@@ -906,7 +920,7 @@
         <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1059,7 +1073,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29">

</xml_diff>